<commit_message>
Fixed constructor of LandingPage.java. Updated ArtifactLocations.java Fixed multiple files
</commit_message>
<xml_diff>
--- a/seleniumPoC/Data Sheet/flipkart.xlsx
+++ b/seleniumPoC/Data Sheet/flipkart.xlsx
@@ -159,12 +159,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -234,15 +234,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="B41" activeCellId="0" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -288,9 +289,6 @@
       <c r="C4" s="0" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>